<commit_message>
added so and pf performing
</commit_message>
<xml_diff>
--- a/src/main/resources/HK list.xlsx
+++ b/src/main/resources/HK list.xlsx
@@ -11,14 +11,14 @@
     <sheet name="suspended" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AK$961</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AK$954</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13622" uniqueCount="4618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13667" uniqueCount="4618">
   <si>
     <t>Company name</t>
   </si>
@@ -14259,8 +14259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK965"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView tabSelected="1" topLeftCell="N921" workbookViewId="0">
+      <selection activeCell="AH944" sqref="AH944"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16819,6 +16819,9 @@
         <v>2425</v>
       </c>
       <c r="Z38" s="3"/>
+      <c r="AI38" t="s">
+        <v>2427</v>
+      </c>
       <c r="AJ38" t="s">
         <v>2425</v>
       </c>
@@ -24542,6 +24545,9 @@
         <v>2425</v>
       </c>
       <c r="Z158" s="3"/>
+      <c r="AI158" t="s">
+        <v>2428</v>
+      </c>
       <c r="AJ158" t="s">
         <v>2425</v>
       </c>
@@ -73209,6 +73215,9 @@
         <v>2425</v>
       </c>
       <c r="Z918" s="3"/>
+      <c r="AI918" t="s">
+        <v>2427</v>
+      </c>
       <c r="AJ918" t="s">
         <v>2425</v>
       </c>
@@ -73258,6 +73267,9 @@
         <v>2425</v>
       </c>
       <c r="Z919" s="3"/>
+      <c r="AI919" t="s">
+        <v>2428</v>
+      </c>
       <c r="AJ919" t="s">
         <v>2425</v>
       </c>
@@ -73356,6 +73368,9 @@
       <c r="AE921" t="s">
         <v>4617</v>
       </c>
+      <c r="AH921" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI921" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73402,6 +73417,9 @@
       <c r="AE922" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH922" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI922" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73448,6 +73466,9 @@
       <c r="AE923" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH923" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI923" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73494,6 +73515,9 @@
       <c r="AE924" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH924" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI924" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73540,6 +73564,9 @@
       <c r="AE925" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH925" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI925" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73586,6 +73613,9 @@
       <c r="AE926" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH926" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI926" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73631,6 +73661,9 @@
       <c r="AE927" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH927" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI927" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73677,6 +73710,9 @@
       <c r="AE928" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH928" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI928" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73723,6 +73759,9 @@
       <c r="AE929" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH929" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI929" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73769,6 +73808,9 @@
       <c r="AE930" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH930" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI930" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73815,6 +73857,9 @@
       <c r="AE931" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH931" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI931" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73861,6 +73906,9 @@
       <c r="AE932" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH932" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI932" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73907,6 +73955,9 @@
       <c r="AE933" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH933" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI933" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73953,6 +74004,9 @@
       <c r="AE934" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH934" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI934" s="8" t="s">
         <v>3116</v>
       </c>
@@ -73999,6 +74053,9 @@
       <c r="AE935" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH935" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI935" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74045,6 +74102,9 @@
       <c r="AE936" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH936" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI936" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74091,6 +74151,9 @@
       <c r="AE937" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH937" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI937" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74137,6 +74200,9 @@
       <c r="AE938" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH938" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI938" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74183,6 +74249,9 @@
       <c r="AE939" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH939" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI939" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74229,6 +74298,9 @@
       <c r="AE940" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH940" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI940" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74275,6 +74347,9 @@
       <c r="AE941" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH941" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI941" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74321,6 +74396,9 @@
       <c r="AE942" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH942" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI942" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74367,6 +74445,9 @@
       <c r="AE943" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH943" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI943" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74413,6 +74494,9 @@
       <c r="AE944" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH944" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI944" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74459,6 +74543,9 @@
       <c r="AE945" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH945" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI945" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74505,6 +74592,9 @@
       <c r="AE946" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH946" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI946" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74551,6 +74641,9 @@
       <c r="AE947" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH947" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI947" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74597,6 +74690,9 @@
       <c r="AE948" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH948" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI948" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74643,6 +74739,9 @@
       <c r="AE949" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH949" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI949" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74689,6 +74788,9 @@
       <c r="AE950" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH950" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI950" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74734,6 +74836,9 @@
       <c r="AE951" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH951" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI951" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74779,6 +74884,9 @@
       <c r="AE952" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH952" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI952" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74824,6 +74932,9 @@
       <c r="AE953" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH953" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI953" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74867,6 +74978,9 @@
       <c r="AE954" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH954" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI954" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74912,6 +75026,9 @@
       <c r="AE955" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH955" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI955" s="8" t="s">
         <v>3116</v>
       </c>
@@ -74957,6 +75074,9 @@
       <c r="AE956" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH956" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI956" s="8" t="s">
         <v>3116</v>
       </c>
@@ -75002,6 +75122,9 @@
       <c r="AE957" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH957" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI957" s="8" t="s">
         <v>3116</v>
       </c>
@@ -75047,6 +75170,9 @@
       <c r="AE958" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH958" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI958" s="8" t="s">
         <v>3116</v>
       </c>
@@ -75092,6 +75218,9 @@
       <c r="AE959" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH959" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI959" s="8" t="s">
         <v>3116</v>
       </c>
@@ -75137,6 +75266,9 @@
       <c r="AE960" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH960" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI960" s="8" t="s">
         <v>3116</v>
       </c>
@@ -75182,6 +75314,9 @@
       <c r="AE961" s="8" t="s">
         <v>4617</v>
       </c>
+      <c r="AH961" s="8" t="s">
+        <v>2425</v>
+      </c>
       <c r="AI961" s="8" t="s">
         <v>3116</v>
       </c>
@@ -75196,7 +75331,7 @@
       <c r="H965" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK961"/>
+  <autoFilter ref="A1:AK954"/>
   <hyperlinks>
     <hyperlink ref="O4" r:id="rId1"/>
     <hyperlink ref="O36" r:id="rId2"/>

</xml_diff>